<commit_message>
update feel gyro page
</commit_message>
<xml_diff>
--- a/images/GYRO/Gen2_BOM.xlsx
+++ b/images/GYRO/Gen2_BOM.xlsx
@@ -5,22 +5,36 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TA1\ugoku-lab.github.io\images\GYRO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/F2AB4736BDF3984A/OneDrive ノートブック/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14DF1E5F-9E0E-4387-BB70-0BAEA476AAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="315" documentId="8_{53329485-A322-45BA-B390-0DE00EFB8790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06CCE426-CF00-4D26-9D3A-AA9446BF8D0F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
   </bookViews>
   <sheets>
-    <sheet name="order" sheetId="1" r:id="rId1"/>
+    <sheet name="fly-wheel_unit" sheetId="2" r:id="rId1"/>
+    <sheet name="misumi_order" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="139">
   <si>
     <t>受注日</t>
   </si>
@@ -301,6 +315,276 @@
   </si>
   <si>
     <t>CSHBTHT-STC-M3-8</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>北日本精機</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>maxon</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>納期(実績)</t>
+    <rPh sb="0" eb="2">
+      <t>ノウキ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ジッセキ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>シャフトホルダ</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>(内製3Dプリント)</t>
+    <rPh sb="1" eb="3">
+      <t>ナイセイ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ベアリング</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ゴムブッシュ</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>六角穴付止めねじ</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>セットカラー</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>インサートナット</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>六角穴付ボタンボルト</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>十字穴付皿小ねじ</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>シムリング</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>フライホイール部品1</t>
+    <rPh sb="7" eb="9">
+      <t>ブヒン</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>フライホイール部品2</t>
+    <rPh sb="7" eb="9">
+      <t>ブヒン</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>SUNCO</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Material</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Supplier</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Part Name</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Balloon Num.</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Part Num.</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>S45C</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>シャフト</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Plating</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Steel</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>S45C相当</t>
+    <rPh sb="4" eb="6">
+      <t>ソウトウ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>CR</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>備考</t>
+    <rPh sb="0" eb="2">
+      <t>ビコウ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>硬度 ショアA65</t>
+    <rPh sb="0" eb="2">
+      <t>コウド</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>SUS304相当</t>
+    <rPh sb="6" eb="8">
+      <t>ソウトウ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>SUS304H</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>SCM</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>黒色酸化被膜</t>
+    <rPh sb="0" eb="6">
+      <t>クロイロサンカヒマク</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>SC0606A</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>A2017</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>FB-3001</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>真鍮 C3604</t>
+    <rPh sb="0" eb="2">
+      <t>シンチュウ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>真鍮</t>
+    <rPh sb="0" eb="2">
+      <t>シンチュウ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>SCM435</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ニッケルメッキ</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>無電解ニッケルメッキ</t>
+    <rPh sb="0" eb="3">
+      <t>ムデンカイ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>PLA</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>BLDC Motor Stator</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>BLDC Motor Roter</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>EC frameless 45 flat 574402</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Unit Price</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>出荷日</t>
+    <rPh sb="0" eb="3">
+      <t>シュッカビ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>meviy使用</t>
+    <rPh sb="5" eb="7">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>フライホイール固定セットカラー</t>
+    <rPh sb="7" eb="9">
+      <t>コテイ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>軸回り止めセットカラー</t>
+    <rPh sb="0" eb="2">
+      <t>ジクマワ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ド</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>(Statorとセット)</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>QTY.</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -308,6 +592,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="5" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -469,7 +756,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -649,8 +936,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -765,6 +1058,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -894,11 +1207,47 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -946,7 +1295,649 @@
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="良い" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="37">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
     </dxf>
@@ -965,6 +1956,60 @@
     <dxf>
       <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -979,15 +2024,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FFB7CF19-F589-4720-8A1E-DB327C1D4AF7}" name="テーブル5" displayName="テーブル5" ref="A1:N18" totalsRowCount="1" headerRowDxfId="36" dataDxfId="35" tableBorderDxfId="34">
+  <autoFilter ref="A1:N17" xr:uid="{FFB7CF19-F589-4720-8A1E-DB327C1D4AF7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N17">
+    <sortCondition ref="A1:A17"/>
+  </sortState>
+  <tableColumns count="14">
+    <tableColumn id="10" xr3:uid="{E69CF2E6-83FB-4B9C-9429-FE67FF73626E}" name="Balloon Num." dataDxfId="27" totalsRowDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{0BA78E67-E02F-49C6-B3C3-A464D2683353}" name="Part Name" dataDxfId="26" totalsRowDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{57E5FC30-C3A3-40B8-B47D-B57C86D62C29}" name="Supplier" dataDxfId="25" totalsRowDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{7E78B8C4-75E6-4641-A05E-82EF8E3B929D}" name="Material" dataDxfId="24" totalsRowDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{CE8FBF84-1ABB-4F3F-B75C-D8642E8824E9}" name="Plating" dataDxfId="23" totalsRowDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{0D709641-BD21-44FA-B07B-F9FA07B1541A}" name="Part Num." dataDxfId="22" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{0E599DBF-9F7B-4B8C-94CC-F6549B320ABC}" name="Unit Price" dataDxfId="21" totalsRowDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{F2125C9E-6857-454C-881F-20E7F8D8D083}" name="QTY." totalsRowLabel="Total" dataDxfId="20" totalsRowDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{C23E117C-F895-4523-ACD7-F882622C49CC}" name="金額(税別)" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="5">
+      <calculatedColumnFormula>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(テーブル5[金額(税別)])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{BD877972-4290-4DB7-8436-2FA932CE41A4}" name="納期(実績)" dataDxfId="18" totalsRowDxfId="4">
+      <calculatedColumnFormula>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="17" xr3:uid="{D0138E4A-910F-4174-8613-2E6458EF2C11}" name="備考" dataDxfId="17" totalsRowDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{4C2E8E32-D666-4B95-925A-8475B68A02B1}" name="消費税" dataDxfId="16" totalsRowDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{9FC65BD9-5248-4133-94E2-BE777088800F}" name="受注日" dataDxfId="15" totalsRowDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{CEC34851-F64E-4ABB-9AE2-6A1B201668D1}" name="出荷日" dataDxfId="14" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C41B289B-18CC-400B-964C-C677741EE5FB}" name="テーブル4" displayName="テーブル4" ref="A1:K37" totalsRowCount="1">
   <autoFilter ref="A1:K36" xr:uid="{C41B289B-18CC-400B-964C-C677741EE5FB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K36">
     <sortCondition ref="K1:K36"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F16D3331-64F7-4EAC-B32A-50FC4B49BE54}" name="受注日" dataDxfId="5" totalsRowDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{162D6D37-3287-427C-ACB9-1584CB52E535}" name="ミスミ出荷日" dataDxfId="4" totalsRowDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{846787E0-9AEF-4953-B5D9-2C6186063A80}" name="メーカー名" dataDxfId="3" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F16D3331-64F7-4EAC-B32A-50FC4B49BE54}" name="受注日" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{162D6D37-3287-427C-ACB9-1584CB52E535}" name="ミスミ出荷日" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{846787E0-9AEF-4953-B5D9-2C6186063A80}" name="メーカー名" dataDxfId="29" totalsRowDxfId="28"/>
     <tableColumn id="2" xr3:uid="{6F12422F-1732-4A01-A0B4-10EEAAFE357F}" name="商品型番"/>
     <tableColumn id="8" xr3:uid="{E14E05B1-2076-4CA6-BE48-4C6BB5EB98A9}" name="商品名称"/>
     <tableColumn id="4" xr3:uid="{DC68FDB4-D2ED-47C5-AB1C-914DD1FBC4A5}" name="単価(税別)"/>
@@ -1319,11 +2395,809 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8338461-2CFA-4B9F-96DC-225D7457421D}">
+  <dimension ref="A1:O21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="15.125" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="21.375" customWidth="1"/>
+    <col min="6" max="6" width="26.25" customWidth="1"/>
+    <col min="7" max="7" width="9.625" customWidth="1"/>
+    <col min="8" max="8" width="5.75" customWidth="1"/>
+    <col min="9" max="9" width="8.875" customWidth="1"/>
+    <col min="10" max="10" width="10.5" customWidth="1"/>
+    <col min="11" max="11" width="14.75" customWidth="1"/>
+    <col min="12" max="12" width="7.375" customWidth="1"/>
+    <col min="13" max="13" width="10.75" customWidth="1"/>
+    <col min="14" max="14" width="11.75" customWidth="1"/>
+    <col min="16" max="16" width="21.875" customWidth="1"/>
+    <col min="17" max="17" width="21.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="9">
+        <v>31000</v>
+      </c>
+      <c r="H2" s="9">
+        <v>1</v>
+      </c>
+      <c r="I2" s="13">
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <v>31000</v>
+      </c>
+      <c r="J2" s="12">
+        <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
+        <v>13</v>
+      </c>
+      <c r="K2" s="12"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="7">
+        <v>45395</v>
+      </c>
+      <c r="N2" s="7">
+        <v>45408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="L3" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="2">
+        <v>16497</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="13">
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <v>16497</v>
+      </c>
+      <c r="J4" s="12">
+        <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
+        <v>17</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1650</v>
+      </c>
+      <c r="M4" s="3">
+        <v>45447</v>
+      </c>
+      <c r="N4" s="3">
+        <v>45464</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="2">
+        <v>22299</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="13">
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <v>22299</v>
+      </c>
+      <c r="J5" s="12">
+        <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
+        <v>16</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="L5" s="2">
+        <v>2230</v>
+      </c>
+      <c r="M5" s="3">
+        <v>45448</v>
+      </c>
+      <c r="N5" s="3">
+        <v>45464</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="2">
+        <v>14169</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="13">
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <v>14169</v>
+      </c>
+      <c r="J6" s="12">
+        <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
+        <v>32</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1417</v>
+      </c>
+      <c r="M6" s="3">
+        <v>45452</v>
+      </c>
+      <c r="N6" s="3">
+        <v>45484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A7" s="6">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="2">
+        <v>609</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2</v>
+      </c>
+      <c r="I7" s="13">
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <v>1218</v>
+      </c>
+      <c r="J7" s="12">
+        <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
+        <v>2</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="2">
+        <v>122</v>
+      </c>
+      <c r="M7" s="3">
+        <v>45459</v>
+      </c>
+      <c r="N7" s="3">
+        <v>45461</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A8" s="6">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="2">
+        <v>590</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="13">
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <v>590</v>
+      </c>
+      <c r="J8" s="12">
+        <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
+        <v>2</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="2">
+        <v>59</v>
+      </c>
+      <c r="M8" s="3">
+        <v>45459</v>
+      </c>
+      <c r="N8" s="3">
+        <v>45461</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A9" s="6">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="2">
+        <v>670</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="13">
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <v>670</v>
+      </c>
+      <c r="J9" s="12">
+        <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
+        <v>5</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="2">
+        <v>67</v>
+      </c>
+      <c r="M9" s="3">
+        <v>45689</v>
+      </c>
+      <c r="N9" s="3">
+        <v>45694</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="2">
+        <v>410</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2</v>
+      </c>
+      <c r="I10" s="13">
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <v>820</v>
+      </c>
+      <c r="J10" s="12">
+        <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
+        <v>4</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L10" s="2">
+        <v>82</v>
+      </c>
+      <c r="M10" s="3">
+        <v>45467</v>
+      </c>
+      <c r="N10" s="3">
+        <v>45471</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="2">
+        <v>21</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1</v>
+      </c>
+      <c r="I11" s="13">
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <v>21</v>
+      </c>
+      <c r="J11" s="12">
+        <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
+        <v>1</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="2">
+        <v>21</v>
+      </c>
+      <c r="M11" s="3">
+        <v>45740</v>
+      </c>
+      <c r="N11" s="3">
+        <v>45741</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" s="9">
+        <v>2</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A13" s="6">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" s="2">
+        <v>251</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2</v>
+      </c>
+      <c r="I13" s="13">
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <v>502</v>
+      </c>
+      <c r="J13" s="12">
+        <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
+        <v>2</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="2">
+        <v>50</v>
+      </c>
+      <c r="M13" s="3">
+        <v>45459</v>
+      </c>
+      <c r="N13" s="3">
+        <v>45461</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A14" s="6">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G14" s="2">
+        <v>21</v>
+      </c>
+      <c r="H14" s="2">
+        <v>6</v>
+      </c>
+      <c r="I14" s="13">
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <v>126</v>
+      </c>
+      <c r="J14" s="12">
+        <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
+        <v>5</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="2">
+        <v>63</v>
+      </c>
+      <c r="M14" s="3">
+        <v>45689</v>
+      </c>
+      <c r="N14" s="3">
+        <v>45694</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A15" s="6">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" s="2">
+        <v>30</v>
+      </c>
+      <c r="H15" s="2">
+        <v>3</v>
+      </c>
+      <c r="I15" s="13">
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <v>90</v>
+      </c>
+      <c r="J15" s="12">
+        <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
+        <v>2</v>
+      </c>
+      <c r="K15" s="5"/>
+      <c r="L15" s="2">
+        <v>30</v>
+      </c>
+      <c r="M15" s="3">
+        <v>45462</v>
+      </c>
+      <c r="N15" s="3">
+        <v>45464</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A16" s="8">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="9">
+        <v>96</v>
+      </c>
+      <c r="H16" s="9">
+        <v>3</v>
+      </c>
+      <c r="I16" s="13">
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <v>288</v>
+      </c>
+      <c r="J16" s="12">
+        <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
+        <v>2</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="L16" s="9">
+        <v>29</v>
+      </c>
+      <c r="M16" s="7">
+        <v>45459</v>
+      </c>
+      <c r="N16" s="7">
+        <v>45461</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A17" s="6">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="2">
+        <v>140</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+      <c r="I17" s="13">
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <v>140</v>
+      </c>
+      <c r="J17" s="12">
+        <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
+        <v>2</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="2">
+        <v>14</v>
+      </c>
+      <c r="M17" s="3">
+        <v>45459</v>
+      </c>
+      <c r="N17" s="3">
+        <v>45461</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="I18" s="13">
+        <f>SUM(テーブル5[金額(税別)])</f>
+        <v>88430</v>
+      </c>
+      <c r="J18" s="6"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="N21" s="9"/>
+      <c r="O21" s="10"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B1A84E-FCD5-4D48-88B5-AF83326CB2F0}">
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
remove top margin from tables to eliminate unexpected gaps
</commit_message>
<xml_diff>
--- a/images/GYRO/Gen2_BOM.xlsx
+++ b/images/GYRO/Gen2_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2ab4736bdf3984a/UGOKU/ugoku-lab.github.io/images/GYRO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="352" documentId="8_{53329485-A322-45BA-B390-0DE00EFB8790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{829429DE-A0DF-4F58-9095-731FBBCA58DE}"/>
+  <xr:revisionPtr revIDLastSave="355" documentId="8_{53329485-A322-45BA-B390-0DE00EFB8790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A28BFD5-08FC-43BA-9403-81617FA5A97A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="141">
   <si>
     <t>受注日</t>
   </si>
@@ -1245,7 +1245,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1274,9 +1274,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
@@ -1336,7 +1333,7 @@
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="良い" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="67">
+  <dxfs count="53">
     <dxf>
       <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1346,226 +1343,6 @@
           <color theme="1"/>
         </top>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1599,6 +1376,17 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1629,469 +1417,14 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
         <top style="thin">
           <color theme="1"/>
         </top>
+        <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2123,6 +1456,81 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2152,6 +1560,16 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2181,6 +1599,16 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2210,6 +1638,60 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2239,6 +1721,16 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2256,6 +1748,7 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2265,6 +1758,16 @@
         <bottom/>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2285,6 +1788,7 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2294,6 +1798,46 @@
         <bottom/>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2415,84 +1959,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2511,58 +1977,24 @@
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
-          <color theme="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2584,14 +2016,24 @@
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
-          <color theme="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2613,14 +2055,24 @@
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
-          <color theme="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2642,38 +2094,24 @@
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
-          <color theme="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2695,14 +2133,24 @@
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
-          <color theme="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2723,16 +2171,25 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
-          <color theme="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2753,16 +2210,103 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
-          <color theme="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2770,6 +2314,9 @@
         <left style="thin">
           <color theme="1"/>
         </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
         <top style="thin">
           <color theme="1"/>
         </top>
@@ -2819,6 +2366,78 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2833,82 +2452,62 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FFB7CF19-F589-4720-8A1E-DB327C1D4AF7}" name="テーブル5" displayName="テーブル5" ref="A1:N18" totalsRowCount="1" headerRowDxfId="66" dataDxfId="65" tableBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FFB7CF19-F589-4720-8A1E-DB327C1D4AF7}" name="テーブル5" displayName="テーブル5" ref="A1:N18" totalsRowCount="1" headerRowDxfId="52" dataDxfId="51" tableBorderDxfId="50">
   <autoFilter ref="A1:N17" xr:uid="{FFB7CF19-F589-4720-8A1E-DB327C1D4AF7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N17">
     <sortCondition ref="A1:A17"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="10" xr3:uid="{E69CF2E6-83FB-4B9C-9429-FE67FF73626E}" name="Balloon Num." dataDxfId="63" totalsRowDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{0BA78E67-E02F-49C6-B3C3-A464D2683353}" name="Part Name" dataDxfId="62" totalsRowDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{57E5FC30-C3A3-40B8-B47D-B57C86D62C29}" name="Supplier" dataDxfId="61" totalsRowDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{7E78B8C4-75E6-4641-A05E-82EF8E3B929D}" name="Material" dataDxfId="60" totalsRowDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{CE8FBF84-1ABB-4F3F-B75C-D8642E8824E9}" name="Plating" dataDxfId="59" totalsRowDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{0D709641-BD21-44FA-B07B-F9FA07B1541A}" name="Part Num." dataDxfId="58" totalsRowDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{0E599DBF-9F7B-4B8C-94CC-F6549B320ABC}" name="Unit Price" dataDxfId="57" totalsRowDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{F2125C9E-6857-454C-881F-20E7F8D8D083}" name="QTY." totalsRowLabel="Total" dataDxfId="56" totalsRowDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{C23E117C-F895-4523-ACD7-F882622C49CC}" name="金額(税別)" totalsRowFunction="custom" dataDxfId="55" totalsRowDxfId="4">
+    <tableColumn id="10" xr3:uid="{E69CF2E6-83FB-4B9C-9429-FE67FF73626E}" name="Balloon Num." dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{0BA78E67-E02F-49C6-B3C3-A464D2683353}" name="Part Name" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{57E5FC30-C3A3-40B8-B47D-B57C86D62C29}" name="Supplier" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="15" xr3:uid="{7E78B8C4-75E6-4641-A05E-82EF8E3B929D}" name="Material" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="16" xr3:uid="{CE8FBF84-1ABB-4F3F-B75C-D8642E8824E9}" name="Plating" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{0D709641-BD21-44FA-B07B-F9FA07B1541A}" name="Part Num." dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{0E599DBF-9F7B-4B8C-94CC-F6549B320ABC}" name="Unit Price" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{F2125C9E-6857-454C-881F-20E7F8D8D083}" name="QTY." totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{C23E117C-F895-4523-ACD7-F882622C49CC}" name="金額(税別)" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="9">
       <calculatedColumnFormula>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(テーブル5[金額(税別)])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BD877972-4290-4DB7-8436-2FA932CE41A4}" name="納期(実績)" dataDxfId="54" totalsRowDxfId="3">
+    <tableColumn id="12" xr3:uid="{BD877972-4290-4DB7-8436-2FA932CE41A4}" name="納期(実績)" dataDxfId="8" totalsRowDxfId="7">
       <calculatedColumnFormula>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{D0138E4A-910F-4174-8613-2E6458EF2C11}" name="備考" dataDxfId="53"/>
-    <tableColumn id="9" xr3:uid="{4C2E8E32-D666-4B95-925A-8475B68A02B1}" name="消費税" dataDxfId="52" totalsRowDxfId="2"/>
-    <tableColumn id="1" xr3:uid="{9FC65BD9-5248-4133-94E2-BE777088800F}" name="受注日" dataDxfId="51" totalsRowDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{CEC34851-F64E-4ABB-9AE2-6A1B201668D1}" name="出荷日" dataDxfId="50" totalsRowDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{D0138E4A-910F-4174-8613-2E6458EF2C11}" name="備考" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{4C2E8E32-D666-4B95-925A-8475B68A02B1}" name="消費税" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{9FC65BD9-5248-4133-94E2-BE777088800F}" name="受注日" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{CEC34851-F64E-4ABB-9AE2-6A1B201668D1}" name="出荷日" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A4B1D07-9A0C-4FFA-BE21-BF1C8C409DC4}" name="テーブル1" displayName="テーブル1" ref="A10:K12" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
-  <autoFilter ref="A10:K12" xr:uid="{5A4B1D07-9A0C-4FFA-BE21-BF1C8C409DC4}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{FF34F2FE-CE2F-4494-B2C2-EF589A47287E}" name="受注日" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{BB4E1D68-1940-414E-99A7-206B1C5F81C9}" name="ミスミ出荷日" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{BD9E5787-B665-4485-B9FF-ECAA193B1056}" name="メーカー名" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{59DD63A4-02E9-4420-A128-570E517A2177}" name="商品型番" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{CF22B847-53C4-49BE-8281-5AE96F91E823}" name="商品名称" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{A3F9C62F-BF20-4192-91A2-B05FB0EC7D0C}" name="単価(税別)" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{03A6F695-15DC-4E7C-A91B-698A35336BF3}" name="数量" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{6F0E9160-367D-4A3F-BA4A-C3D6986351CA}" name="金額(税別)" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{C7A3B729-4AE2-4AB0-A841-AC0E85A83B69}" name="消費税" dataDxfId="35"/>
-    <tableColumn id="10" xr3:uid="{39DD7BA6-70CF-4E18-8548-F5E956045858}" name="原産国" dataDxfId="34"/>
-    <tableColumn id="11" xr3:uid="{A2CF466E-56AF-4BCC-AD2D-7B0BBAF7E7AD}" name="分類" dataDxfId="33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}" name="テーブル3" displayName="テーブル3" ref="A1:N4" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" tableBorderDxfId="41">
+  <autoFilter ref="A1:N4" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{C1C0B2C7-9798-40C8-AD09-A6827F915F22}" name="Balloon" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{1CE48C0A-22FF-488A-9A7E-B73356A27B12}" name="Part Name" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{D674320C-FA0C-423F-AB87-E1B5C58FE2F9}" name="Supplier" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{C55C935A-BCE3-4CE1-9105-78B5680DD98F}" name="Material" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{68EA2C49-E7D0-46AF-993F-99385E39AAFC}" name="Plating" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{9D74A4A7-39C8-49A3-B00B-0FC0479180CB}" name="Part Num." dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{65A21D04-56DC-42BB-BF94-4B99024FA621}" name="Unit Price" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{12791772-E497-4361-9D88-68395E68291F}" name="QTY." dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{FCBEA251-2FA5-4901-9F9A-E4325C78EB9F}" name="金額(税別)" dataDxfId="27">
+      <calculatedColumnFormula>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY.]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{B604651F-FBED-4C66-90D8-26CA3506AD10}" name="納期(実績)" dataDxfId="34"/>
+    <tableColumn id="11" xr3:uid="{71E5A3E7-2DDC-4D5C-9DC1-9D3783AB63E3}" name="備考" dataDxfId="33"/>
+    <tableColumn id="12" xr3:uid="{E824A542-547E-4145-864D-24CA4DB4EBD3}" name="消費税" dataDxfId="32"/>
+    <tableColumn id="13" xr3:uid="{DFAB695D-55D8-4628-9072-10089F337DBD}" name="受注日" dataDxfId="31"/>
+    <tableColumn id="14" xr3:uid="{5EE5CB39-33D3-4188-929E-0C812CC100E2}" name="出荷日" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}" name="テーブル3" displayName="テーブル3" ref="A1:N4" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
-  <autoFilter ref="A1:N4" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{C1C0B2C7-9798-40C8-AD09-A6827F915F22}" name="Balloon" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{1CE48C0A-22FF-488A-9A7E-B73356A27B12}" name="Part Name" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{D674320C-FA0C-423F-AB87-E1B5C58FE2F9}" name="Supplier" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{C55C935A-BCE3-4CE1-9105-78B5680DD98F}" name="Material" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{68EA2C49-E7D0-46AF-993F-99385E39AAFC}" name="Plating" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{9D74A4A7-39C8-49A3-B00B-0FC0479180CB}" name="Part Num." dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{65A21D04-56DC-42BB-BF94-4B99024FA621}" name="Unit Price" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{12791772-E497-4361-9D88-68395E68291F}" name="QTY." dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{FCBEA251-2FA5-4901-9F9A-E4325C78EB9F}" name="金額(税別)" dataDxfId="13">
-      <calculatedColumnFormula>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY.]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="10" xr3:uid="{B604651F-FBED-4C66-90D8-26CA3506AD10}" name="納期(実績)" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{71E5A3E7-2DDC-4D5C-9DC1-9D3783AB63E3}" name="備考" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{E824A542-547E-4145-864D-24CA4DB4EBD3}" name="消費税" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{DFAB695D-55D8-4628-9072-10089F337DBD}" name="受注日" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{5EE5CB39-33D3-4188-929E-0C812CC100E2}" name="出荷日" dataDxfId="16"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C41B289B-18CC-400B-964C-C677741EE5FB}" name="テーブル4" displayName="テーブル4" ref="A1:K37" totalsRowCount="1">
   <autoFilter ref="A1:K36" xr:uid="{C41B289B-18CC-400B-964C-C677741EE5FB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K36">
@@ -3265,8 +2864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8338461-2CFA-4B9F-96DC-225D7457421D}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4052,10 +3651,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E2BF92-DA56-4BCB-B8B4-7CEAABB467D1}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4114,15 +3713,15 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A2" s="11"/>
+      <c r="A2" s="10"/>
       <c r="B2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
       <c r="F2" s="7" t="s">
         <v>21</v>
       </c>
@@ -4132,13 +3731,13 @@
       <c r="H2" s="7">
         <v>32</v>
       </c>
-      <c r="I2" s="12">
+      <c r="I2" s="11">
         <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY.]]</f>
         <v>672</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
       <c r="M2" s="8">
         <v>45689</v>
       </c>
@@ -4147,15 +3746,15 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A3" s="11"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="7" t="s">
         <v>23</v>
       </c>
@@ -4165,13 +3764,13 @@
       <c r="H3" s="7">
         <v>10</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="11">
         <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY.]]</f>
         <v>180</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
       <c r="M3" s="8">
         <v>45689</v>
       </c>
@@ -4180,133 +3779,31 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A4" s="13"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="14">
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13">
         <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY.]]</f>
         <v>0</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A10" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A11" s="8">
-        <v>45689</v>
-      </c>
-      <c r="B11" s="8">
-        <v>45694</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="7">
-        <v>21</v>
-      </c>
-      <c r="G11" s="7">
-        <v>32</v>
-      </c>
-      <c r="H11" s="7">
-        <v>672</v>
-      </c>
-      <c r="I11" s="7">
-        <v>67</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A12" s="8">
-        <v>45689</v>
-      </c>
-      <c r="B12" s="8">
-        <v>45694</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="7">
-        <v>18</v>
-      </c>
-      <c r="G12" s="7">
-        <v>10</v>
-      </c>
-      <c r="H12" s="7">
-        <v>180</v>
-      </c>
-      <c r="I12" s="7">
-        <v>18</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>81</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="1">
     <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
update BOM column definitions and enhance currency formatting for unit prices
</commit_message>
<xml_diff>
--- a/images/GYRO/Gen2_BOM.xlsx
+++ b/images/GYRO/Gen2_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2ab4736bdf3984a/UGOKU/ugoku-lab.github.io/images/GYRO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="355" documentId="8_{53329485-A322-45BA-B390-0DE00EFB8790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A28BFD5-08FC-43BA-9403-81617FA5A97A}"/>
+  <xr:revisionPtr revIDLastSave="397" documentId="8_{53329485-A322-45BA-B390-0DE00EFB8790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFB30DC9-65ED-40AB-8847-C11A995260F1}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="4" r:id="rId1"/>
@@ -328,16 +328,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>納期(実績)</t>
-    <rPh sb="0" eb="2">
-      <t>ノウキ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ジッセキ</t>
-    </rPh>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>シャフトホルダ</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -411,27 +401,11 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>Part Name</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Balloon Num.</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Part Num.</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>S45C</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
     <t>シャフト</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Plating</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
@@ -447,13 +421,6 @@
   </si>
   <si>
     <t>CR</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>備考</t>
-    <rPh sb="0" eb="2">
-      <t>ビコウ</t>
-    </rPh>
     <phoneticPr fontId="18"/>
   </si>
   <si>
@@ -586,15 +553,39 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>QTY.</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>Balloon</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
     <t>F6700ZZ</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Partname</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Surface Finishing</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Part Number</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>QTY</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Price</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Lead Time</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Note</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -1346,6 +1337,157 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1376,17 +1518,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1417,16 +1548,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1459,28 +1580,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -1521,16 +1621,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1560,16 +1650,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1599,16 +1679,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1638,16 +1708,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1660,16 +1720,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1679,55 +1729,6 @@
         <bottom/>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1761,16 +1762,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2458,25 +2449,25 @@
     <sortCondition ref="A1:A17"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="10" xr3:uid="{E69CF2E6-83FB-4B9C-9429-FE67FF73626E}" name="Balloon Num." dataDxfId="26" totalsRowDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{0BA78E67-E02F-49C6-B3C3-A464D2683353}" name="Part Name" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{57E5FC30-C3A3-40B8-B47D-B57C86D62C29}" name="Supplier" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="15" xr3:uid="{7E78B8C4-75E6-4641-A05E-82EF8E3B929D}" name="Material" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="16" xr3:uid="{CE8FBF84-1ABB-4F3F-B75C-D8642E8824E9}" name="Plating" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{0D709641-BD21-44FA-B07B-F9FA07B1541A}" name="Part Num." dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{0E599DBF-9F7B-4B8C-94CC-F6549B320ABC}" name="Unit Price" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{F2125C9E-6857-454C-881F-20E7F8D8D083}" name="QTY." totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{C23E117C-F895-4523-ACD7-F882622C49CC}" name="金額(税別)" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="9">
-      <calculatedColumnFormula>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</calculatedColumnFormula>
-      <totalsRowFormula>SUM(テーブル5[金額(税別)])</totalsRowFormula>
+    <tableColumn id="10" xr3:uid="{E69CF2E6-83FB-4B9C-9429-FE67FF73626E}" name="Balloon" dataDxfId="26" totalsRowDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{0BA78E67-E02F-49C6-B3C3-A464D2683353}" name="Partname" dataDxfId="25" totalsRowDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{7E78B8C4-75E6-4641-A05E-82EF8E3B929D}" name="Material" dataDxfId="24" totalsRowDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{CE8FBF84-1ABB-4F3F-B75C-D8642E8824E9}" name="Surface Finishing" dataDxfId="23" totalsRowDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{0D709641-BD21-44FA-B07B-F9FA07B1541A}" name="Part Number" dataDxfId="22" totalsRowDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{57E5FC30-C3A3-40B8-B47D-B57C86D62C29}" name="Supplier" dataDxfId="13" totalsRowDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{0E599DBF-9F7B-4B8C-94CC-F6549B320ABC}" name="Unit Price" dataDxfId="21" totalsRowDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{F2125C9E-6857-454C-881F-20E7F8D8D083}" name="QTY" totalsRowLabel="Total" dataDxfId="20" totalsRowDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{C23E117C-F895-4523-ACD7-F882622C49CC}" name="Price" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="4">
+      <calculatedColumnFormula>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(テーブル5[Price])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BD877972-4290-4DB7-8436-2FA932CE41A4}" name="納期(実績)" dataDxfId="8" totalsRowDxfId="7">
+    <tableColumn id="12" xr3:uid="{BD877972-4290-4DB7-8436-2FA932CE41A4}" name="Lead Time" dataDxfId="18" totalsRowDxfId="3">
       <calculatedColumnFormula>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{D0138E4A-910F-4174-8613-2E6458EF2C11}" name="備考" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{4C2E8E32-D666-4B95-925A-8475B68A02B1}" name="消費税" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{9FC65BD9-5248-4133-94E2-BE777088800F}" name="受注日" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{CEC34851-F64E-4ABB-9AE2-6A1B201668D1}" name="出荷日" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{D0138E4A-910F-4174-8613-2E6458EF2C11}" name="Note" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{4C2E8E32-D666-4B95-925A-8475B68A02B1}" name="消費税" dataDxfId="16" totalsRowDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{9FC65BD9-5248-4133-94E2-BE777088800F}" name="受注日" dataDxfId="15" totalsRowDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{CEC34851-F64E-4ABB-9AE2-6A1B201668D1}" name="出荷日" dataDxfId="14" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2487,18 +2478,18 @@
   <autoFilter ref="A1:N4" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{C1C0B2C7-9798-40C8-AD09-A6827F915F22}" name="Balloon" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{1CE48C0A-22FF-488A-9A7E-B73356A27B12}" name="Part Name" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{D674320C-FA0C-423F-AB87-E1B5C58FE2F9}" name="Supplier" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{C55C935A-BCE3-4CE1-9105-78B5680DD98F}" name="Material" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{68EA2C49-E7D0-46AF-993F-99385E39AAFC}" name="Plating" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{9D74A4A7-39C8-49A3-B00B-0FC0479180CB}" name="Part Num." dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{1CE48C0A-22FF-488A-9A7E-B73356A27B12}" name="Partname" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{D674320C-FA0C-423F-AB87-E1B5C58FE2F9}" name="Material" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{C55C935A-BCE3-4CE1-9105-78B5680DD98F}" name="Surface Finishing" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{68EA2C49-E7D0-46AF-993F-99385E39AAFC}" name="Part Number" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{9D74A4A7-39C8-49A3-B00B-0FC0479180CB}" name="Supplier" dataDxfId="29"/>
     <tableColumn id="7" xr3:uid="{65A21D04-56DC-42BB-BF94-4B99024FA621}" name="Unit Price" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{12791772-E497-4361-9D88-68395E68291F}" name="QTY." dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{FCBEA251-2FA5-4901-9F9A-E4325C78EB9F}" name="金額(税別)" dataDxfId="27">
-      <calculatedColumnFormula>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY.]]</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{12791772-E497-4361-9D88-68395E68291F}" name="QTY" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{FCBEA251-2FA5-4901-9F9A-E4325C78EB9F}" name="Price" dataDxfId="27">
+      <calculatedColumnFormula>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{B604651F-FBED-4C66-90D8-26CA3506AD10}" name="納期(実績)" dataDxfId="34"/>
-    <tableColumn id="11" xr3:uid="{71E5A3E7-2DDC-4D5C-9DC1-9D3783AB63E3}" name="備考" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{B604651F-FBED-4C66-90D8-26CA3506AD10}" name="Lead Time" dataDxfId="34"/>
+    <tableColumn id="11" xr3:uid="{71E5A3E7-2DDC-4D5C-9DC1-9D3783AB63E3}" name="Note" dataDxfId="33"/>
     <tableColumn id="12" xr3:uid="{E824A542-547E-4145-864D-24CA4DB4EBD3}" name="消費税" dataDxfId="32"/>
     <tableColumn id="13" xr3:uid="{DFAB695D-55D8-4628-9072-10089F337DBD}" name="受注日" dataDxfId="31"/>
     <tableColumn id="14" xr3:uid="{5EE5CB39-33D3-4188-929E-0C812CC100E2}" name="出荷日" dataDxfId="30"/>
@@ -2862,65 +2853,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8338461-2CFA-4B9F-96DC-225D7457421D}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="3" max="3" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="18.875" customWidth="1"/>
     <col min="5" max="5" width="21.375" customWidth="1"/>
-    <col min="6" max="6" width="26.25" customWidth="1"/>
-    <col min="7" max="7" width="9.625" customWidth="1"/>
-    <col min="8" max="8" width="5.75" customWidth="1"/>
-    <col min="9" max="9" width="8.875" customWidth="1"/>
-    <col min="10" max="10" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="14.75" customWidth="1"/>
-    <col min="12" max="12" width="7.375" customWidth="1"/>
-    <col min="13" max="13" width="10.75" customWidth="1"/>
-    <col min="14" max="14" width="11.75" customWidth="1"/>
-    <col min="16" max="16" width="21.875" customWidth="1"/>
-    <col min="17" max="17" width="21.625" customWidth="1"/>
+    <col min="6" max="6" width="16.375" customWidth="1"/>
+    <col min="7" max="8" width="11.5" customWidth="1"/>
+    <col min="9" max="9" width="8.25" customWidth="1"/>
+    <col min="10" max="10" width="13.625" customWidth="1"/>
+    <col min="11" max="11" width="12.625" customWidth="1"/>
+    <col min="12" max="12" width="14.75" customWidth="1"/>
+    <col min="13" max="13" width="7.375" customWidth="1"/>
+    <col min="14" max="14" width="10.75" customWidth="1"/>
+    <col min="15" max="15" width="11.75" customWidth="1"/>
+    <col min="17" max="17" width="21.875" customWidth="1"/>
+    <col min="18" max="18" width="21.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>106</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="J1" s="4" t="s">
-        <v>87</v>
+        <v>139</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>5</v>
@@ -2929,7 +2920,7 @@
         <v>0</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
@@ -2937,19 +2928,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="G2" s="2">
         <v>31000</v>
@@ -2958,7 +2949,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="6">
-        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
         <v>31000</v>
       </c>
       <c r="J2">
@@ -2978,35 +2969,35 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -3016,19 +3007,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="G4" s="2">
         <v>16497</v>
@@ -3037,7 +3028,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="6">
-        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
         <v>16497</v>
       </c>
       <c r="J4">
@@ -3045,7 +3036,7 @@
         <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="L4" s="2">
         <v>1650</v>
@@ -3062,19 +3053,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="G5" s="2">
         <v>22299</v>
@@ -3083,7 +3074,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="6">
-        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
         <v>22299</v>
       </c>
       <c r="J5">
@@ -3091,7 +3082,7 @@
         <v>16</v>
       </c>
       <c r="K5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="L5" s="2">
         <v>2230</v>
@@ -3108,19 +3099,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="G6" s="2">
         <v>14169</v>
@@ -3129,7 +3120,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="6">
-        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
         <v>14169</v>
       </c>
       <c r="J6">
@@ -3137,7 +3128,7 @@
         <v>32</v>
       </c>
       <c r="K6" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="L6" s="2">
         <v>1417</v>
@@ -3154,19 +3145,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="G7" s="2">
         <v>609</v>
@@ -3175,7 +3166,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="6">
-        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
         <v>1218</v>
       </c>
       <c r="J7">
@@ -3197,19 +3188,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="G8" s="2">
         <v>590</v>
@@ -3218,7 +3209,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="6">
-        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
         <v>590</v>
       </c>
       <c r="J8">
@@ -3240,19 +3231,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="G9" s="2">
         <v>670</v>
@@ -3261,7 +3252,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="6">
-        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
         <v>670</v>
       </c>
       <c r="J9">
@@ -3283,19 +3274,19 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="G10" s="2">
         <v>410</v>
@@ -3304,7 +3295,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="6">
-        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
         <v>820</v>
       </c>
       <c r="J10">
@@ -3312,7 +3303,7 @@
         <v>4</v>
       </c>
       <c r="K10" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="L10" s="2">
         <v>82</v>
@@ -3329,19 +3320,19 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>118</v>
+        <v>17</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="G11" s="2">
         <v>21</v>
@@ -3350,7 +3341,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="6">
-        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
         <v>21</v>
       </c>
       <c r="J11">
@@ -3372,39 +3363,39 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
         <v>89</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H12" s="2">
         <v>2</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.4">
@@ -3412,17 +3403,17 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="G13" s="2">
         <v>251</v>
@@ -3431,7 +3422,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="6">
-        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
         <v>502</v>
       </c>
       <c r="J13">
@@ -3453,17 +3444,17 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="G14" s="2">
         <v>21</v>
@@ -3472,7 +3463,7 @@
         <v>6</v>
       </c>
       <c r="I14" s="6">
-        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
         <v>126</v>
       </c>
       <c r="J14">
@@ -3494,19 +3485,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="G15" s="2">
         <v>30</v>
@@ -3515,7 +3506,7 @@
         <v>3</v>
       </c>
       <c r="I15" s="6">
-        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
         <v>90</v>
       </c>
       <c r="J15">
@@ -3537,17 +3528,17 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="G16" s="2">
         <v>96</v>
@@ -3556,7 +3547,7 @@
         <v>3</v>
       </c>
       <c r="I16" s="6">
-        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
         <v>288</v>
       </c>
       <c r="J16">
@@ -3574,22 +3565,22 @@
         <v>45461</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" s="2">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="G17" s="2">
         <v>140</v>
@@ -3598,7 +3589,7 @@
         <v>1</v>
       </c>
       <c r="I17" s="6">
-        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY.]]</f>
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
         <v>140</v>
       </c>
       <c r="J17">
@@ -3616,7 +3607,7 @@
         <v>45461</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3625,10 +3616,10 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="I18" s="6">
-        <f>SUM(テーブル5[金額(税別)])</f>
+        <f>SUM(テーブル5[Price])</f>
         <v>88430</v>
       </c>
       <c r="J18" s="2"/>
@@ -3636,9 +3627,9 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="N21" s="2"/>
-      <c r="O21" s="5"/>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="O21" s="2"/>
+      <c r="P21" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>
@@ -3653,8 +3644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E2BF92-DA56-4BCB-B8B4-7CEAABB467D1}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3669,38 +3660,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>113</v>
+      <c r="K1" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>5</v>
@@ -3709,7 +3700,7 @@
         <v>0</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
@@ -3732,7 +3723,7 @@
         <v>32</v>
       </c>
       <c r="I2" s="11">
-        <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY.]]</f>
+        <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
         <v>672</v>
       </c>
       <c r="J2" s="10"/>
@@ -3765,7 +3756,7 @@
         <v>10</v>
       </c>
       <c r="I3" s="11">
-        <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY.]]</f>
+        <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
         <v>180</v>
       </c>
       <c r="J3" s="10"/>
@@ -3790,7 +3781,7 @@
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="13">
-        <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY.]]</f>
+        <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
         <v>0</v>
       </c>
       <c r="J4" s="12"/>
@@ -3802,8 +3793,9 @@
   </sheetData>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
adjust padding for table cells in main.css for improved layout
</commit_message>
<xml_diff>
--- a/images/GYRO/Gen2_BOM.xlsx
+++ b/images/GYRO/Gen2_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2ab4736bdf3984a/UGOKU/ugoku-lab.github.io/images/GYRO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="397" documentId="8_{53329485-A322-45BA-B390-0DE00EFB8790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFB30DC9-65ED-40AB-8847-C11A995260F1}"/>
+  <xr:revisionPtr revIDLastSave="401" documentId="8_{53329485-A322-45BA-B390-0DE00EFB8790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6227447E-E688-4650-8FE0-323FD157FEA0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="141">
   <si>
     <t>受注日</t>
   </si>
@@ -944,7 +944,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1107,6 +1107,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1236,7 +1249,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1277,6 +1290,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="5" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2855,8 +2871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8338461-2CFA-4B9F-96DC-225D7457421D}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2981,7 +2997,7 @@
         <v>130</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>88</v>
@@ -3644,8 +3660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E2BF92-DA56-4BCB-B8B4-7CEAABB467D1}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3708,13 +3724,13 @@
       <c r="B2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="G2" s="7">
         <v>21</v>
@@ -3741,13 +3757,13 @@
       <c r="B3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="G3" s="7">
         <v>18</v>
@@ -3772,9 +3788,7 @@
     <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" s="12"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="12" t="s">
-        <v>13</v>
-      </c>
+      <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="7"/>

</xml_diff>

<commit_message>
update table cell padding and enforce text alignment for BOM table columns
</commit_message>
<xml_diff>
--- a/images/GYRO/Gen2_BOM.xlsx
+++ b/images/GYRO/Gen2_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2ab4736bdf3984a/UGOKU/ugoku-lab.github.io/images/GYRO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="401" documentId="8_{53329485-A322-45BA-B390-0DE00EFB8790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6227447E-E688-4650-8FE0-323FD157FEA0}"/>
+  <xr:revisionPtr revIDLastSave="409" documentId="8_{53329485-A322-45BA-B390-0DE00EFB8790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9924993-EF34-4A40-BAFA-C6C84314FA82}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="4" r:id="rId1"/>
@@ -483,17 +483,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>ニッケルメッキ</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>無電解ニッケルメッキ</t>
-    <rPh sb="0" eb="3">
-      <t>ムデンカイ</t>
-    </rPh>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>PLA</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -524,13 +513,6 @@
     <t>meviy使用</t>
     <rPh sb="5" eb="7">
       <t>シヨウ</t>
-    </rPh>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>フライホイール固定セットカラー</t>
-    <rPh sb="7" eb="9">
-      <t>コテイ</t>
     </rPh>
     <phoneticPr fontId="18"/>
   </si>
@@ -586,6 +568,24 @@
   </si>
   <si>
     <t>Note</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>無電解ﾆｯｹﾙﾒｯｷ</t>
+    <rPh sb="0" eb="3">
+      <t>ムデンカイ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ﾆｯｹﾙﾒｯｷ</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ﾌﾗｲﾎｲｰﾙ固定ｾｯﾄｶﾗｰ</t>
+    <rPh sb="7" eb="9">
+      <t>コテイ</t>
+    </rPh>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -2871,8 +2871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8338461-2CFA-4B9F-96DC-225D7457421D}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2897,37 +2897,37 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>102</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>5</v>
@@ -2936,7 +2936,7 @@
         <v>0</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
@@ -2944,7 +2944,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>88</v>
@@ -2953,7 +2953,7 @@
         <v>88</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>86</v>
@@ -2985,7 +2985,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>88</v>
@@ -2994,7 +2994,7 @@
         <v>88</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>88</v>
@@ -3029,7 +3029,7 @@
         <v>103</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>75</v>
@@ -3052,7 +3052,7 @@
         <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L4" s="2">
         <v>1650</v>
@@ -3098,7 +3098,7 @@
         <v>16</v>
       </c>
       <c r="K5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L5" s="2">
         <v>2230</v>
@@ -3144,7 +3144,7 @@
         <v>32</v>
       </c>
       <c r="K6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L6" s="2">
         <v>1417</v>
@@ -3170,7 +3170,7 @@
         <v>88</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>85</v>
@@ -3204,13 +3204,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>106</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>70</v>
@@ -3247,13 +3247,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>106</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>38</v>
@@ -3382,7 +3382,7 @@
         <v>87</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
@@ -3507,7 +3507,7 @@
         <v>118</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>83</v>
@@ -3632,7 +3632,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="I18" s="6">
         <f>SUM(テーブル5[Price])</f>
@@ -3660,7 +3660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E2BF92-DA56-4BCB-B8B4-7CEAABB467D1}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -3677,37 +3677,37 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>102</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>5</v>
@@ -3716,7 +3716,7 @@
         <v>0</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
add BOM table for system components and enhance data fetching logic
</commit_message>
<xml_diff>
--- a/images/GYRO/Gen2_BOM.xlsx
+++ b/images/GYRO/Gen2_BOM.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2ab4736bdf3984a/UGOKU/ugoku-lab.github.io/images/GYRO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="409" documentId="8_{53329485-A322-45BA-B390-0DE00EFB8790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9924993-EF34-4A40-BAFA-C6C84314FA82}"/>
+  <xr:revisionPtr revIDLastSave="428" documentId="8_{53329485-A322-45BA-B390-0DE00EFB8790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50719C42-E871-4D51-A8FF-7CA1103011A9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
   </bookViews>
   <sheets>
-    <sheet name="System" sheetId="4" r:id="rId1"/>
+    <sheet name="system" sheetId="4" r:id="rId1"/>
     <sheet name="fly-wheel_unit" sheetId="2" r:id="rId2"/>
     <sheet name="enclosure" sheetId="3" r:id="rId3"/>
     <sheet name="misumi_order" sheetId="1" r:id="rId4"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="141">
   <si>
     <t>受注日</t>
   </si>
@@ -944,7 +944,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1081,6 +1081,17 @@
     </border>
     <border>
       <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -1249,7 +1260,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1274,18 +1285,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="5" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1293,6 +1304,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2856,12 +2873,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36ED456B-82D0-46D1-973B-1463394C28CD}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="3" max="3" width="13.25" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="15.125" customWidth="1"/>
+    <col min="6" max="6" width="11.875" customWidth="1"/>
+    <col min="7" max="7" width="15.75" customWidth="1"/>
+    <col min="8" max="8" width="11.625" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2871,8 +2956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8338461-2CFA-4B9F-96DC-225D7457421D}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3709,27 +3794,27 @@
       <c r="K1" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="11" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A2" s="10"/>
+      <c r="A2" s="12"/>
       <c r="B2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="10"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="12"/>
       <c r="E2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="7">
@@ -3738,31 +3823,31 @@
       <c r="H2" s="7">
         <v>32</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="13">
         <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
         <v>672</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="8">
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="10">
         <v>45689</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="10">
         <v>45694</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A3" s="10"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="14" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="7">
@@ -3771,38 +3856,38 @@
       <c r="H3" s="7">
         <v>10</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="13">
         <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
         <v>180</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="8">
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="10">
         <v>45689</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="10">
         <v>45694</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A4" s="12"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="13">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15">
         <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
         <v>0</v>
       </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>

</xml_diff>

<commit_message>
Enhance image display in rotor media section and update BOM file
</commit_message>
<xml_diff>
--- a/images/GYRO/Gen2_BOM.xlsx
+++ b/images/GYRO/Gen2_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2ab4736bdf3984a/UGOKU/ugoku-lab.github.io/images/GYRO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="430" documentId="8_{53329485-A322-45BA-B390-0DE00EFB8790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{935CFEA3-9606-4729-B973-5EC1A4FEADFB}"/>
+  <xr:revisionPtr revIDLastSave="442" documentId="8_{53329485-A322-45BA-B390-0DE00EFB8790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EB74CEE-FBB8-4D89-94DC-EEF6D3334CEC}"/>
   <bookViews>
-    <workbookView xWindow="1635" yWindow="3525" windowWidth="21600" windowHeight="9960" activeTab="1" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
   </bookViews>
   <sheets>
     <sheet name="system" sheetId="4" r:id="rId1"/>
@@ -1270,7 +1270,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1320,6 +1320,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2966,8 +2969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8338461-2CFA-4B9F-96DC-225D7457421D}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3114,8 +3117,8 @@
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A4" s="2">
-        <v>2</v>
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>104</v>
@@ -3161,7 +3164,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>98</v>
@@ -3206,8 +3209,8 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A6" s="2">
-        <v>4</v>
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>99</v>
@@ -3253,7 +3256,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>90</v>
@@ -3295,40 +3298,39 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A8" s="2">
-        <v>6</v>
+      <c r="A8" s="17">
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>140</v>
+        <v>97</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>138</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="2">
-        <v>590</v>
+        <v>140</v>
       </c>
       <c r="H8" s="2">
         <v>1</v>
       </c>
       <c r="I8" s="6">
         <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
-        <v>590</v>
+        <v>140</v>
       </c>
       <c r="J8">
         <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
         <v>2</v>
       </c>
+      <c r="K8" s="17"/>
       <c r="L8" s="2">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="M8" s="3">
         <v>45459</v>
@@ -3339,10 +3341,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>106</v>
@@ -3351,371 +3353,374 @@
         <v>138</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="2">
-        <v>670</v>
+        <v>590</v>
       </c>
       <c r="H9" s="2">
         <v>1</v>
       </c>
       <c r="I9" s="6">
         <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
-        <v>670</v>
+        <v>590</v>
       </c>
       <c r="J9">
         <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L9" s="2">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="M9" s="3">
-        <v>45689</v>
+        <v>45459</v>
       </c>
       <c r="N9" s="3">
-        <v>45694</v>
+        <v>45461</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A10" s="2">
-        <v>8</v>
+      <c r="A10" s="17">
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="2">
-        <v>410</v>
+        <v>670</v>
       </c>
       <c r="H10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10" s="6">
         <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
-        <v>820</v>
+        <v>670</v>
       </c>
       <c r="J10">
         <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
-        <v>4</v>
-      </c>
-      <c r="K10" t="s">
-        <v>108</v>
+        <v>5</v>
       </c>
       <c r="L10" s="2">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="M10" s="3">
-        <v>45467</v>
+        <v>45689</v>
       </c>
       <c r="N10" s="3">
-        <v>45471</v>
+        <v>45694</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>112</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="G11" s="2">
-        <v>21</v>
+        <v>251</v>
       </c>
       <c r="H11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" s="6">
         <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
-        <v>21</v>
+        <v>502</v>
       </c>
       <c r="J11">
         <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11" s="2">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="M11" s="3">
-        <v>45740</v>
+        <v>45459</v>
       </c>
       <c r="N11" s="3">
-        <v>45741</v>
+        <v>45461</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A12" s="2">
-        <v>10</v>
+      <c r="A12">
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>107</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="E12" s="2" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>88</v>
+        <v>11</v>
+      </c>
+      <c r="G12" s="2">
+        <v>410</v>
       </c>
       <c r="H12" s="2">
         <v>2</v>
       </c>
-      <c r="I12" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="J12" t="s">
-        <v>88</v>
-      </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>88</v>
+      <c r="I12" s="6">
+        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
+        <v>820</v>
+      </c>
+      <c r="J12">
+        <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
+        <v>4</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="L12" s="2">
+        <v>82</v>
+      </c>
+      <c r="M12" s="3">
+        <v>45467</v>
+      </c>
+      <c r="N12" s="3">
+        <v>45471</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G13" s="2">
-        <v>251</v>
+        <v>89</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="H13" s="2">
         <v>2</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J13" t="s">
+        <v>88</v>
+      </c>
+      <c r="K13" s="17"/>
+      <c r="L13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A14" s="17">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="2">
+        <v>30</v>
+      </c>
+      <c r="H14" s="2">
+        <v>3</v>
+      </c>
+      <c r="I14" s="6">
         <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
-        <v>502</v>
-      </c>
-      <c r="J13">
+        <v>90</v>
+      </c>
+      <c r="J14">
         <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
         <v>2</v>
       </c>
-      <c r="L13" s="2">
-        <v>50</v>
-      </c>
-      <c r="M13" s="3">
-        <v>45459</v>
-      </c>
-      <c r="N13" s="3">
-        <v>45461</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A14" s="2">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F14" s="2" t="s">
+      <c r="L14" s="2">
         <v>30</v>
       </c>
-      <c r="G14" s="2">
-        <v>21</v>
-      </c>
-      <c r="H14" s="2">
-        <v>6</v>
-      </c>
-      <c r="I14" s="6">
-        <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
-        <v>126</v>
-      </c>
-      <c r="J14">
-        <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
-        <v>5</v>
-      </c>
-      <c r="L14" s="2">
-        <v>63</v>
-      </c>
       <c r="M14" s="3">
-        <v>45689</v>
+        <v>45462</v>
       </c>
       <c r="N14" s="3">
-        <v>45694</v>
+        <v>45464</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>139</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="G15" s="2">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="H15" s="2">
         <v>3</v>
       </c>
       <c r="I15" s="6">
         <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
-        <v>90</v>
+        <v>288</v>
       </c>
       <c r="J15">
         <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
         <v>2</v>
       </c>
+      <c r="K15" s="17"/>
       <c r="L15" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M15" s="3">
-        <v>45462</v>
+        <v>45459</v>
       </c>
       <c r="N15" s="3">
-        <v>45464</v>
+        <v>45461</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A16" s="2">
-        <v>14</v>
+      <c r="A16" s="17">
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D16" s="2"/>
+        <v>111</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="E16" s="2" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="G16" s="2">
-        <v>96</v>
+        <v>21</v>
       </c>
       <c r="H16" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I16" s="6">
         <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
-        <v>288</v>
+        <v>21</v>
       </c>
       <c r="J16">
         <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="M16" s="3">
-        <v>45459</v>
+        <v>45740</v>
       </c>
       <c r="N16" s="3">
-        <v>45461</v>
+        <v>45741</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>57</v>
+        <v>115</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G17" s="2">
-        <v>140</v>
+        <v>21</v>
       </c>
       <c r="H17" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I17" s="6">
         <f>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</f>
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="J17">
         <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="M17" s="3">
-        <v>45459</v>
+        <v>45689</v>
       </c>
       <c r="N17" s="3">
-        <v>45461</v>
+        <v>45694</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
add fly-wheel asm steps
</commit_message>
<xml_diff>
--- a/images/GYRO/Gen2_BOM.xlsx
+++ b/images/GYRO/Gen2_BOM.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2ab4736bdf3984a/UGOKU/ugoku-lab.github.io/images/GYRO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="442" documentId="8_{53329485-A322-45BA-B390-0DE00EFB8790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EB74CEE-FBB8-4D89-94DC-EEF6D3334CEC}"/>
+  <xr:revisionPtr revIDLastSave="484" documentId="8_{53329485-A322-45BA-B390-0DE00EFB8790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F69D447-9482-4B7A-ABD6-065AF8B7554C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
+    <workbookView minimized="1" xWindow="1635" yWindow="3525" windowWidth="21600" windowHeight="9960" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
   </bookViews>
   <sheets>
-    <sheet name="system" sheetId="4" r:id="rId1"/>
-    <sheet name="fly-wheel_unit" sheetId="2" r:id="rId2"/>
-    <sheet name="enclosure" sheetId="3" r:id="rId3"/>
+    <sheet name="fly-wheel_unit" sheetId="2" r:id="rId1"/>
+    <sheet name="enclosure" sheetId="3" r:id="rId2"/>
+    <sheet name="system" sheetId="4" r:id="rId3"/>
     <sheet name="misumi_order" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="160">
   <si>
     <t>受注日</t>
   </si>
@@ -595,6 +595,121 @@
     </rPh>
     <rPh sb="8" eb="10">
       <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>UI Board</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>BMS Board</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>M5 Stick C Plus2</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Battery</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Efest</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>https://www.efestpower.com/index.php?ac=article&amp;at=read&amp;did=550</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Desgin</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Fusion</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Spec</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>1200mAh 10A</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>INR 18350</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>HXYP-C47-MA18</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>https://www.tztstore.com/goods/show-7668.html</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Link</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>MotorDriver Board</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>KiCad</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>JunctionBoard</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">BMS IC </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>深圳市创芯微微电子股份有限公司製</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CM1361</t>
+    </r>
+    <rPh sb="22" eb="23">
+      <t>セイ</t>
     </rPh>
     <phoneticPr fontId="18"/>
   </si>
@@ -606,7 +721,7 @@
   <numFmts count="1">
     <numFmt numFmtId="5" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -765,6 +880,29 @@
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1142,7 +1280,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1269,8 +1407,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1325,8 +1466,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - アクセント 1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - アクセント 2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - アクセント 3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1354,6 +1498,7 @@
     <cellStyle name="タイトル" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="チェック セル" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="どちらでもない" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="ハイパーリンク" xfId="42" builtinId="8"/>
     <cellStyle name="メモ" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="リンク セル" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="悪い" xfId="7" builtinId="27" customBuiltin="1"/>
@@ -1370,7 +1515,32 @@
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="良い" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="54">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -2489,71 +2659,92 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FFB7CF19-F589-4720-8A1E-DB327C1D4AF7}" name="テーブル5" displayName="テーブル5" ref="A1:N18" totalsRowCount="1" headerRowDxfId="52" dataDxfId="51" tableBorderDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FFB7CF19-F589-4720-8A1E-DB327C1D4AF7}" name="テーブル5" displayName="テーブル5" ref="A1:N18" totalsRowCount="1" headerRowDxfId="53" dataDxfId="52" tableBorderDxfId="51">
   <autoFilter ref="A1:N17" xr:uid="{FFB7CF19-F589-4720-8A1E-DB327C1D4AF7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N17">
     <sortCondition ref="A1:A17"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="10" xr3:uid="{E69CF2E6-83FB-4B9C-9429-FE67FF73626E}" name="Balloon" dataDxfId="26" totalsRowDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{0BA78E67-E02F-49C6-B3C3-A464D2683353}" name="Partname" dataDxfId="25" totalsRowDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{7E78B8C4-75E6-4641-A05E-82EF8E3B929D}" name="Material" dataDxfId="24" totalsRowDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{CE8FBF84-1ABB-4F3F-B75C-D8642E8824E9}" name="Surface Finishing" dataDxfId="23" totalsRowDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{0D709641-BD21-44FA-B07B-F9FA07B1541A}" name="Part Number" dataDxfId="22" totalsRowDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{57E5FC30-C3A3-40B8-B47D-B57C86D62C29}" name="Supplier" dataDxfId="13" totalsRowDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{0E599DBF-9F7B-4B8C-94CC-F6549B320ABC}" name="Unit Price" dataDxfId="21" totalsRowDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{F2125C9E-6857-454C-881F-20E7F8D8D083}" name="QTY" totalsRowLabel="Total" dataDxfId="20" totalsRowDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{C23E117C-F895-4523-ACD7-F882622C49CC}" name="Price" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="4">
+    <tableColumn id="10" xr3:uid="{E69CF2E6-83FB-4B9C-9429-FE67FF73626E}" name="Balloon" dataDxfId="27" totalsRowDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{0BA78E67-E02F-49C6-B3C3-A464D2683353}" name="Partname" dataDxfId="26" totalsRowDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{7E78B8C4-75E6-4641-A05E-82EF8E3B929D}" name="Material" dataDxfId="25" totalsRowDxfId="11"/>
+    <tableColumn id="16" xr3:uid="{CE8FBF84-1ABB-4F3F-B75C-D8642E8824E9}" name="Surface Finishing" dataDxfId="24" totalsRowDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{0D709641-BD21-44FA-B07B-F9FA07B1541A}" name="Part Number" dataDxfId="23" totalsRowDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{57E5FC30-C3A3-40B8-B47D-B57C86D62C29}" name="Supplier" dataDxfId="14" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{0E599DBF-9F7B-4B8C-94CC-F6549B320ABC}" name="Unit Price" dataDxfId="22" totalsRowDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{F2125C9E-6857-454C-881F-20E7F8D8D083}" name="QTY" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{C23E117C-F895-4523-ACD7-F882622C49CC}" name="Price" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="5">
       <calculatedColumnFormula>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(テーブル5[Price])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BD877972-4290-4DB7-8436-2FA932CE41A4}" name="Lead Time" dataDxfId="18" totalsRowDxfId="3">
+    <tableColumn id="12" xr3:uid="{BD877972-4290-4DB7-8436-2FA932CE41A4}" name="Lead Time" dataDxfId="19" totalsRowDxfId="4">
       <calculatedColumnFormula>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{D0138E4A-910F-4174-8613-2E6458EF2C11}" name="Note" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{4C2E8E32-D666-4B95-925A-8475B68A02B1}" name="消費税" dataDxfId="16" totalsRowDxfId="2"/>
-    <tableColumn id="1" xr3:uid="{9FC65BD9-5248-4133-94E2-BE777088800F}" name="受注日" dataDxfId="15" totalsRowDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{CEC34851-F64E-4ABB-9AE2-6A1B201668D1}" name="出荷日" dataDxfId="14" totalsRowDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{D0138E4A-910F-4174-8613-2E6458EF2C11}" name="Note" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{4C2E8E32-D666-4B95-925A-8475B68A02B1}" name="消費税" dataDxfId="17" totalsRowDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{9FC65BD9-5248-4133-94E2-BE777088800F}" name="受注日" dataDxfId="16" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{CEC34851-F64E-4ABB-9AE2-6A1B201668D1}" name="出荷日" dataDxfId="15" totalsRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}" name="テーブル3" displayName="テーブル3" ref="A1:N4" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" tableBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}" name="テーブル3" displayName="テーブル3" ref="A1:N4" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" tableBorderDxfId="42">
   <autoFilter ref="A1:N4" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{C1C0B2C7-9798-40C8-AD09-A6827F915F22}" name="Balloon" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{1CE48C0A-22FF-488A-9A7E-B73356A27B12}" name="Partname" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{D674320C-FA0C-423F-AB87-E1B5C58FE2F9}" name="Material" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{C55C935A-BCE3-4CE1-9105-78B5680DD98F}" name="Surface Finishing" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{68EA2C49-E7D0-46AF-993F-99385E39AAFC}" name="Part Number" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{9D74A4A7-39C8-49A3-B00B-0FC0479180CB}" name="Supplier" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{65A21D04-56DC-42BB-BF94-4B99024FA621}" name="Unit Price" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{12791772-E497-4361-9D88-68395E68291F}" name="QTY" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{FCBEA251-2FA5-4901-9F9A-E4325C78EB9F}" name="Price" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{C1C0B2C7-9798-40C8-AD09-A6827F915F22}" name="Balloon" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{1CE48C0A-22FF-488A-9A7E-B73356A27B12}" name="Partname" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{D674320C-FA0C-423F-AB87-E1B5C58FE2F9}" name="Material" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{C55C935A-BCE3-4CE1-9105-78B5680DD98F}" name="Surface Finishing" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{68EA2C49-E7D0-46AF-993F-99385E39AAFC}" name="Part Number" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{9D74A4A7-39C8-49A3-B00B-0FC0479180CB}" name="Supplier" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{65A21D04-56DC-42BB-BF94-4B99024FA621}" name="Unit Price" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{12791772-E497-4361-9D88-68395E68291F}" name="QTY" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{FCBEA251-2FA5-4901-9F9A-E4325C78EB9F}" name="Price" dataDxfId="28">
       <calculatedColumnFormula>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{B604651F-FBED-4C66-90D8-26CA3506AD10}" name="Lead Time" dataDxfId="34"/>
-    <tableColumn id="11" xr3:uid="{71E5A3E7-2DDC-4D5C-9DC1-9D3783AB63E3}" name="Note" dataDxfId="33"/>
-    <tableColumn id="12" xr3:uid="{E824A542-547E-4145-864D-24CA4DB4EBD3}" name="消費税" dataDxfId="32"/>
-    <tableColumn id="13" xr3:uid="{DFAB695D-55D8-4628-9072-10089F337DBD}" name="受注日" dataDxfId="31"/>
-    <tableColumn id="14" xr3:uid="{5EE5CB39-33D3-4188-929E-0C812CC100E2}" name="出荷日" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{B604651F-FBED-4C66-90D8-26CA3506AD10}" name="Lead Time" dataDxfId="35"/>
+    <tableColumn id="11" xr3:uid="{71E5A3E7-2DDC-4D5C-9DC1-9D3783AB63E3}" name="Note" dataDxfId="34"/>
+    <tableColumn id="12" xr3:uid="{E824A542-547E-4145-864D-24CA4DB4EBD3}" name="消費税" dataDxfId="33"/>
+    <tableColumn id="13" xr3:uid="{DFAB695D-55D8-4628-9072-10089F337DBD}" name="受注日" dataDxfId="32"/>
+    <tableColumn id="14" xr3:uid="{5EE5CB39-33D3-4188-929E-0C812CC100E2}" name="出荷日" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A0CBC9AA-8108-43DE-9508-48638514B39D}" name="テーブル6" displayName="テーブル6" ref="A1:L11" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:L11" xr:uid="{A0CBC9AA-8108-43DE-9508-48638514B39D}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{19CFD427-1401-4365-870F-C15308F7351E}" name="Balloon"/>
+    <tableColumn id="2" xr3:uid="{CD11486A-628E-4733-A0D9-D030643514AF}" name="Partname"/>
+    <tableColumn id="3" xr3:uid="{9D163939-F08D-48F2-A476-278A1208D01C}" name="Desgin"/>
+    <tableColumn id="4" xr3:uid="{7E92743D-B709-4181-AF07-A94DBB48DC7D}" name="Spec"/>
+    <tableColumn id="5" xr3:uid="{756F00E9-4BD2-449D-B059-EA4D001BA88B}" name="Part Number"/>
+    <tableColumn id="6" xr3:uid="{288F36DF-7E11-40A2-86ED-6B4484317D63}" name="Supplier"/>
+    <tableColumn id="7" xr3:uid="{D3EBE681-7399-4F2D-BE92-D76AF1BF02F0}" name="Unit Price"/>
+    <tableColumn id="8" xr3:uid="{02D5FADE-D644-45C6-AB9B-1F0F4AA44B54}" name="QTY"/>
+    <tableColumn id="9" xr3:uid="{76AAA32C-1419-4C8C-B97D-1AB00A84F966}" name="Price"/>
+    <tableColumn id="10" xr3:uid="{7EAAA854-7F61-4DD7-A7BA-4EE9FEB91922}" name="Lead Time"/>
+    <tableColumn id="12" xr3:uid="{06195832-326E-4080-B08A-4265083EA1A3}" name="Note"/>
+    <tableColumn id="11" xr3:uid="{3334C49F-AA41-4B2B-BE88-E74FBB38A99E}" name="Link"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C41B289B-18CC-400B-964C-C677741EE5FB}" name="テーブル4" displayName="テーブル4" ref="A1:K37" totalsRowCount="1">
   <autoFilter ref="A1:K36" xr:uid="{C41B289B-18CC-400B-964C-C677741EE5FB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K36">
     <sortCondition ref="K1:K36"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F16D3331-64F7-4EAC-B32A-50FC4B49BE54}" name="受注日" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{162D6D37-3287-427C-ACB9-1584CB52E535}" name="ミスミ出荷日" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="9" xr3:uid="{846787E0-9AEF-4953-B5D9-2C6186063A80}" name="メーカー名" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{F16D3331-64F7-4EAC-B32A-50FC4B49BE54}" name="受注日" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{162D6D37-3287-427C-ACB9-1584CB52E535}" name="ミスミ出荷日" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="9" xr3:uid="{846787E0-9AEF-4953-B5D9-2C6186063A80}" name="メーカー名" dataDxfId="46" totalsRowDxfId="45"/>
     <tableColumn id="2" xr3:uid="{6F12422F-1732-4A01-A0B4-10EEAAFE357F}" name="商品型番"/>
     <tableColumn id="8" xr3:uid="{E14E05B1-2076-4CA6-BE48-4C6BB5EB98A9}" name="商品名称"/>
     <tableColumn id="4" xr3:uid="{DC68FDB4-D2ED-47C5-AB1C-914DD1FBC4A5}" name="単価(税別)"/>
@@ -2885,87 +3076,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36ED456B-82D0-46D1-973B-1463394C28CD}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="13.75" customWidth="1"/>
-    <col min="3" max="3" width="13.25" customWidth="1"/>
-    <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="15.125" customWidth="1"/>
-    <col min="6" max="6" width="11.875" customWidth="1"/>
-    <col min="7" max="7" width="15.75" customWidth="1"/>
-    <col min="8" max="8" width="11.625" customWidth="1"/>
-    <col min="10" max="10" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A5">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="18"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8338461-2CFA-4B9F-96DC-225D7457421D}">
   <dimension ref="A1:P21"/>
   <sheetViews>
@@ -3756,7 +3866,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E2BF92-DA56-4BCB-B8B4-7CEAABB467D1}">
   <dimension ref="A1:N4"/>
   <sheetViews>
@@ -3910,6 +4020,162 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36ED456B-82D0-46D1-973B-1463394C28CD}">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="9.625" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="13.25" customWidth="1"/>
+    <col min="4" max="5" width="25.75" customWidth="1"/>
+    <col min="6" max="6" width="10.25" customWidth="1"/>
+    <col min="7" max="7" width="11.75" customWidth="1"/>
+    <col min="8" max="8" width="11.625" customWidth="1"/>
+    <col min="10" max="10" width="6.5" customWidth="1"/>
+    <col min="11" max="11" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A1" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>159</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" t="s">
+        <v>146</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18"/>
+  <hyperlinks>
+    <hyperlink ref="L5" r:id="rId1" xr:uid="{CB1C367E-A921-4281-96DA-DFF15C62CFF3}"/>
+    <hyperlink ref="L4" r:id="rId2" xr:uid="{26752813-B826-4419-9EA6-1B2E3D3E288E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
update bom, feelgyro page
</commit_message>
<xml_diff>
--- a/images/GYRO/Gen2_BOM.xlsx
+++ b/images/GYRO/Gen2_BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2ab4736bdf3984a/UGOKU/ugoku-lab.github.io/images/GYRO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TA1\ugoku-lab.github.io\images\GYRO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="484" documentId="8_{53329485-A322-45BA-B390-0DE00EFB8790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F69D447-9482-4B7A-ABD6-065AF8B7554C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A62692-76DA-4448-8E45-969AAAEF4544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1635" yWindow="3525" windowWidth="21600" windowHeight="9960" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
   </bookViews>
   <sheets>
     <sheet name="fly-wheel_unit" sheetId="2" r:id="rId1"/>
@@ -675,27 +675,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">BMS IC </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>深圳市创芯微微电子股份有限公司製</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve">BMS IC: iCM </t>
     </r>
     <r>
       <rPr>
@@ -708,9 +688,6 @@
       </rPr>
       <t>CM1361</t>
     </r>
-    <rPh sb="22" eb="23">
-      <t>セイ</t>
-    </rPh>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -721,7 +698,7 @@
   <numFmts count="1">
     <numFmt numFmtId="5" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -889,13 +866,6 @@
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Microsoft YaHei"/>
-      <family val="2"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1411,7 +1381,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1433,37 +1403,25 @@
     <xf numFmtId="5" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="5" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="5" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42">
@@ -1517,6 +1475,24 @@
   </cellStyles>
   <dxfs count="54">
     <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1540,570 +1516,6 @@
           <bgColor theme="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -2300,6 +1712,7 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2418,6 +1831,35 @@
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -2475,6 +1917,74 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2575,21 +2085,469 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2665,57 +2623,57 @@
     <sortCondition ref="A1:A17"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="10" xr3:uid="{E69CF2E6-83FB-4B9C-9429-FE67FF73626E}" name="Balloon" dataDxfId="27" totalsRowDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{0BA78E67-E02F-49C6-B3C3-A464D2683353}" name="Partname" dataDxfId="26" totalsRowDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{7E78B8C4-75E6-4641-A05E-82EF8E3B929D}" name="Material" dataDxfId="25" totalsRowDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{CE8FBF84-1ABB-4F3F-B75C-D8642E8824E9}" name="Surface Finishing" dataDxfId="24" totalsRowDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{0D709641-BD21-44FA-B07B-F9FA07B1541A}" name="Part Number" dataDxfId="23" totalsRowDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{57E5FC30-C3A3-40B8-B47D-B57C86D62C29}" name="Supplier" dataDxfId="14" totalsRowDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{0E599DBF-9F7B-4B8C-94CC-F6549B320ABC}" name="Unit Price" dataDxfId="22" totalsRowDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{F2125C9E-6857-454C-881F-20E7F8D8D083}" name="QTY" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{C23E117C-F895-4523-ACD7-F882622C49CC}" name="Price" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="5">
+    <tableColumn id="10" xr3:uid="{E69CF2E6-83FB-4B9C-9429-FE67FF73626E}" name="Balloon" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{0BA78E67-E02F-49C6-B3C3-A464D2683353}" name="Partname" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="15" xr3:uid="{7E78B8C4-75E6-4641-A05E-82EF8E3B929D}" name="Material" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="16" xr3:uid="{CE8FBF84-1ABB-4F3F-B75C-D8642E8824E9}" name="Surface Finishing" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{0D709641-BD21-44FA-B07B-F9FA07B1541A}" name="Part Number" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{57E5FC30-C3A3-40B8-B47D-B57C86D62C29}" name="Supplier" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{0E599DBF-9F7B-4B8C-94CC-F6549B320ABC}" name="Unit Price" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{F2125C9E-6857-454C-881F-20E7F8D8D083}" name="QTY" totalsRowLabel="Total" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{C23E117C-F895-4523-ACD7-F882622C49CC}" name="Price" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="33">
       <calculatedColumnFormula>テーブル5[[#This Row],[Unit Price]]*テーブル5[[#This Row],[QTY]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(テーブル5[Price])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BD877972-4290-4DB7-8436-2FA932CE41A4}" name="Lead Time" dataDxfId="19" totalsRowDxfId="4">
+    <tableColumn id="12" xr3:uid="{BD877972-4290-4DB7-8436-2FA932CE41A4}" name="Lead Time" dataDxfId="32" totalsRowDxfId="31">
       <calculatedColumnFormula>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{D0138E4A-910F-4174-8613-2E6458EF2C11}" name="Note" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{4C2E8E32-D666-4B95-925A-8475B68A02B1}" name="消費税" dataDxfId="17" totalsRowDxfId="3"/>
-    <tableColumn id="1" xr3:uid="{9FC65BD9-5248-4133-94E2-BE777088800F}" name="受注日" dataDxfId="16" totalsRowDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{CEC34851-F64E-4ABB-9AE2-6A1B201668D1}" name="出荷日" dataDxfId="15" totalsRowDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{D0138E4A-910F-4174-8613-2E6458EF2C11}" name="Note" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{4C2E8E32-D666-4B95-925A-8475B68A02B1}" name="消費税" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{9FC65BD9-5248-4133-94E2-BE777088800F}" name="受注日" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{CEC34851-F64E-4ABB-9AE2-6A1B201668D1}" name="出荷日" dataDxfId="25" totalsRowDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}" name="テーブル3" displayName="テーブル3" ref="A1:N4" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" tableBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}" name="テーブル3" displayName="テーブル3" ref="A1:N4" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
   <autoFilter ref="A1:N4" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{C1C0B2C7-9798-40C8-AD09-A6827F915F22}" name="Balloon" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{1CE48C0A-22FF-488A-9A7E-B73356A27B12}" name="Partname" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{D674320C-FA0C-423F-AB87-E1B5C58FE2F9}" name="Material" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{C55C935A-BCE3-4CE1-9105-78B5680DD98F}" name="Surface Finishing" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{68EA2C49-E7D0-46AF-993F-99385E39AAFC}" name="Part Number" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{9D74A4A7-39C8-49A3-B00B-0FC0479180CB}" name="Supplier" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{65A21D04-56DC-42BB-BF94-4B99024FA621}" name="Unit Price" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{12791772-E497-4361-9D88-68395E68291F}" name="QTY" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{FCBEA251-2FA5-4901-9F9A-E4325C78EB9F}" name="Price" dataDxfId="28">
+    <tableColumn id="1" xr3:uid="{C1C0B2C7-9798-40C8-AD09-A6827F915F22}" name="Balloon" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{1CE48C0A-22FF-488A-9A7E-B73356A27B12}" name="Partname" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{D674320C-FA0C-423F-AB87-E1B5C58FE2F9}" name="Material" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{C55C935A-BCE3-4CE1-9105-78B5680DD98F}" name="Surface Finishing" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{68EA2C49-E7D0-46AF-993F-99385E39AAFC}" name="Part Number" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{9D74A4A7-39C8-49A3-B00B-0FC0479180CB}" name="Supplier" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{65A21D04-56DC-42BB-BF94-4B99024FA621}" name="Unit Price" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{12791772-E497-4361-9D88-68395E68291F}" name="QTY" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{FCBEA251-2FA5-4901-9F9A-E4325C78EB9F}" name="Price" dataDxfId="12">
       <calculatedColumnFormula>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{B604651F-FBED-4C66-90D8-26CA3506AD10}" name="Lead Time" dataDxfId="35"/>
-    <tableColumn id="11" xr3:uid="{71E5A3E7-2DDC-4D5C-9DC1-9D3783AB63E3}" name="Note" dataDxfId="34"/>
-    <tableColumn id="12" xr3:uid="{E824A542-547E-4145-864D-24CA4DB4EBD3}" name="消費税" dataDxfId="33"/>
-    <tableColumn id="13" xr3:uid="{DFAB695D-55D8-4628-9072-10089F337DBD}" name="受注日" dataDxfId="32"/>
-    <tableColumn id="14" xr3:uid="{5EE5CB39-33D3-4188-929E-0C812CC100E2}" name="出荷日" dataDxfId="31"/>
+    <tableColumn id="10" xr3:uid="{B604651F-FBED-4C66-90D8-26CA3506AD10}" name="Lead Time" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{71E5A3E7-2DDC-4D5C-9DC1-9D3783AB63E3}" name="Note" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{E824A542-547E-4145-864D-24CA4DB4EBD3}" name="消費税" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{DFAB695D-55D8-4628-9072-10089F337DBD}" name="受注日" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{5EE5CB39-33D3-4188-929E-0C812CC100E2}" name="出荷日" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A0CBC9AA-8108-43DE-9508-48638514B39D}" name="テーブル6" displayName="テーブル6" ref="A1:L11" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A0CBC9AA-8108-43DE-9508-48638514B39D}" name="テーブル6" displayName="テーブル6" ref="A1:L11" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:L11" xr:uid="{A0CBC9AA-8108-43DE-9508-48638514B39D}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{19CFD427-1401-4365-870F-C15308F7351E}" name="Balloon"/>
@@ -2742,9 +2700,9 @@
     <sortCondition ref="K1:K36"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F16D3331-64F7-4EAC-B32A-50FC4B49BE54}" name="受注日" dataDxfId="50" totalsRowDxfId="49"/>
-    <tableColumn id="7" xr3:uid="{162D6D37-3287-427C-ACB9-1584CB52E535}" name="ミスミ出荷日" dataDxfId="48" totalsRowDxfId="47"/>
-    <tableColumn id="9" xr3:uid="{846787E0-9AEF-4953-B5D9-2C6186063A80}" name="メーカー名" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{F16D3331-64F7-4EAC-B32A-50FC4B49BE54}" name="受注日" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{162D6D37-3287-427C-ACB9-1584CB52E535}" name="ミスミ出荷日" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{846787E0-9AEF-4953-B5D9-2C6186063A80}" name="メーカー名" dataDxfId="1" totalsRowDxfId="0"/>
     <tableColumn id="2" xr3:uid="{6F12422F-1732-4A01-A0B4-10EEAAFE357F}" name="商品型番"/>
     <tableColumn id="8" xr3:uid="{E14E05B1-2076-4CA6-BE48-4C6BB5EB98A9}" name="商品名称"/>
     <tableColumn id="4" xr3:uid="{DC68FDB4-D2ED-47C5-AB1C-914DD1FBC4A5}" name="単価(税別)"/>
@@ -3079,7 +3037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8338461-2CFA-4B9F-96DC-225D7457421D}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -3408,7 +3366,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A8" s="17">
+      <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -3438,7 +3396,6 @@
         <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
         <v>2</v>
       </c>
-      <c r="K8" s="17"/>
       <c r="L8" s="2">
         <v>14</v>
       </c>
@@ -3493,7 +3450,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A10" s="17">
+      <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -3651,7 +3608,6 @@
       <c r="J13" t="s">
         <v>88</v>
       </c>
-      <c r="K13" s="17"/>
       <c r="L13" s="2" t="s">
         <v>88</v>
       </c>
@@ -3663,7 +3619,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A14" s="17">
+      <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -3736,7 +3692,6 @@
         <f>-_xlfn.DAYS(テーブル5[[#This Row],[受注日]],テーブル5[[#This Row],[出荷日]])</f>
         <v>2</v>
       </c>
-      <c r="K15" s="17"/>
       <c r="L15" s="2">
         <v>29</v>
       </c>
@@ -3748,7 +3703,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A16" s="17">
+      <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -3919,100 +3874,100 @@
       <c r="K1" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="4" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A2" s="12"/>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="7" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="2">
         <v>21</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="2">
         <v>32</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="10">
         <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
         <v>672</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="10">
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="3">
         <v>45689</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="3">
         <v>45694</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A3" s="12"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="7" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="2">
         <v>18</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="2">
         <v>10</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="10">
         <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
         <v>180</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="10">
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="3">
         <v>45689</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="3">
         <v>45694</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A4" s="14"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="15">
+      <c r="A4" s="11"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12">
         <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
         <v>0</v>
       </c>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>
@@ -4028,8 +3983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36ED456B-82D0-46D1-973B-1463394C28CD}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4046,40 +4001,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>136</v>
       </c>
       <c r="K1" t="s">
         <v>137</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4118,7 +4073,7 @@
       <c r="K4" t="s">
         <v>159</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="14" t="s">
         <v>154</v>
       </c>
     </row>
@@ -4141,7 +4096,7 @@
       <c r="H5">
         <v>6</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="L5" s="14" t="s">
         <v>147</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add BOM enclosure pannel
</commit_message>
<xml_diff>
--- a/images/GYRO/Gen2_BOM.xlsx
+++ b/images/GYRO/Gen2_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TA1\ugoku-lab.github.io\images\GYRO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A62692-76DA-4448-8E45-969AAAEF4544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E103D04B-1B6C-434C-9EC4-243399DE6AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
   </bookViews>
   <sheets>
     <sheet name="fly-wheel_unit" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="172">
   <si>
     <t>受注日</t>
   </si>
@@ -690,15 +690,63 @@
     </r>
     <phoneticPr fontId="18"/>
   </si>
+  <si>
+    <t>Motor Driver: Maxon DECModule
+ 50/5  380200</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>https://www.maxongroup.co.jp/maxon/view/product/380200</t>
+  </si>
+  <si>
+    <t>ポリカーボネート</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>JLCCNC</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Vapor polishing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Enclosure panel buttom</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Enclosure panel top</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Enclosure panel side L</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Enclosure panel side R</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Enclosure panel side Rr</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Enclosure panel side Fr</t>
+    <phoneticPr fontId="18"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="5" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
+    <numFmt numFmtId="183" formatCode="\$#,##0.00;\-\$#,##0.00"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -873,6 +921,14 @@
       <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1381,7 +1437,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1425,6 +1481,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2648,8 +2719,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}" name="テーブル3" displayName="テーブル3" ref="A1:N4" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
-  <autoFilter ref="A1:N4" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}" name="テーブル3" displayName="テーブル3" ref="A1:N10" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
+  <autoFilter ref="A1:N10" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{C1C0B2C7-9798-40C8-AD09-A6827F915F22}" name="Balloon" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{1CE48C0A-22FF-488A-9A7E-B73356A27B12}" name="Partname" dataDxfId="19"/>
@@ -3823,16 +3894,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E2BF92-DA56-4BCB-B8B4-7CEAABB467D1}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="12.125" customWidth="1"/>
     <col min="4" max="4" width="10.375" customWidth="1"/>
     <col min="5" max="5" width="10.25" customWidth="1"/>
@@ -3886,26 +3957,28 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="9"/>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2">
-        <v>21</v>
-      </c>
-      <c r="H2" s="2">
-        <v>32</v>
-      </c>
-      <c r="I2" s="10">
+      <c r="B2" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="G2" s="18">
+        <v>25.58</v>
+      </c>
+      <c r="H2" s="17">
+        <v>1</v>
+      </c>
+      <c r="I2" s="19">
         <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
-        <v>672</v>
+        <v>25.58</v>
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
@@ -3919,55 +3992,244 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" s="9"/>
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>13</v>
+      <c r="B3" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="16" t="s">
+        <v>163</v>
       </c>
       <c r="G3" s="2">
-        <v>18</v>
+        <v>19.98</v>
       </c>
       <c r="H3" s="2">
-        <v>10</v>
-      </c>
-      <c r="I3" s="10">
+        <v>1</v>
+      </c>
+      <c r="I3" s="19">
         <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
-        <v>180</v>
+        <v>19.98</v>
       </c>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
-      <c r="M3" s="3">
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A4" s="9"/>
+      <c r="B4" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="G4" s="2">
+        <v>26.15</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="19">
+        <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
+        <v>26.15</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A5" s="9"/>
+      <c r="B5" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="G5" s="2">
+        <v>22.7</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="19">
+        <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
+        <v>22.7</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A6" s="9"/>
+      <c r="B6" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="G6" s="2">
+        <v>22.56</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="19">
+        <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
+        <v>22.56</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A7" s="9"/>
+      <c r="B7" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="G7" s="2">
+        <v>23.85</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="19">
+        <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
+        <v>23.85</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A8" s="9"/>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2">
+        <v>21</v>
+      </c>
+      <c r="H8" s="2">
+        <v>32</v>
+      </c>
+      <c r="I8" s="10">
+        <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
+        <v>672</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A9" s="9"/>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="2">
+        <v>18</v>
+      </c>
+      <c r="H9" s="2">
+        <v>10</v>
+      </c>
+      <c r="I9" s="10">
+        <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
+        <v>180</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="3">
         <v>45689</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N9" s="3">
         <v>45694</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A4" s="11"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="12">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A10" s="11"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12">
         <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
         <v>0</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G18" t="s">
+        <v>165</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>
@@ -3983,8 +4245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36ED456B-82D0-46D1-973B-1463394C28CD}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4100,7 +4362,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4109,6 +4371,12 @@
       </c>
       <c r="C6" t="s">
         <v>157</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="L6" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
update gyro enclosure bom
</commit_message>
<xml_diff>
--- a/images/GYRO/Gen2_BOM.xlsx
+++ b/images/GYRO/Gen2_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TA1\ugoku-lab.github.io\images\GYRO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB628ADF-E536-4228-842B-7F9FAAA4B6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77E6EC4-A163-4030-8F04-C9C8A0615F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{0936869C-9685-4355-9997-2DA68DFC34DD}"/>
   </bookViews>
@@ -1452,7 +1452,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1516,9 +1516,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="183" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1529,6 +1526,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="5" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="21" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1579,25 +1582,328 @@
   </cellStyles>
   <dxfs count="55">
     <dxf>
-      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1623,6 +1929,9 @@
           <bgColor theme="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
     </dxf>
     <dxf>
       <font>
@@ -1842,328 +2151,22 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
     </dxf>
     <dxf>
       <font>
@@ -2755,35 +2758,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}" name="テーブル3" displayName="テーブル3" ref="A1:O10" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}" name="テーブル3" displayName="テーブル3" ref="A1:O10" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A1:O10" xr:uid="{B31FBE47-1031-43AC-AB6B-77ABDF2834D1}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{C1C0B2C7-9798-40C8-AD09-A6827F915F22}" name="Balloon" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{1CE48C0A-22FF-488A-9A7E-B73356A27B12}" name="Partname" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{D674320C-FA0C-423F-AB87-E1B5C58FE2F9}" name="Material" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{C55C935A-BCE3-4CE1-9105-78B5680DD98F}" name="Surface Finishing" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{68EA2C49-E7D0-46AF-993F-99385E39AAFC}" name="Part Number" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{9D74A4A7-39C8-49A3-B00B-0FC0479180CB}" name="Supplier" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{65A21D04-56DC-42BB-BF94-4B99024FA621}" name="Unit Price" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{12791772-E497-4361-9D88-68395E68291F}" name="QTY" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{FCBEA251-2FA5-4901-9F9A-E4325C78EB9F}" name="Price" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{C1C0B2C7-9798-40C8-AD09-A6827F915F22}" name="Balloon" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{1CE48C0A-22FF-488A-9A7E-B73356A27B12}" name="Partname" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{D674320C-FA0C-423F-AB87-E1B5C58FE2F9}" name="Material" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{C55C935A-BCE3-4CE1-9105-78B5680DD98F}" name="Surface Finishing" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{68EA2C49-E7D0-46AF-993F-99385E39AAFC}" name="Part Number" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{9D74A4A7-39C8-49A3-B00B-0FC0479180CB}" name="Supplier" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{65A21D04-56DC-42BB-BF94-4B99024FA621}" name="Unit Price" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{12791772-E497-4361-9D88-68395E68291F}" name="QTY" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{FCBEA251-2FA5-4901-9F9A-E4325C78EB9F}" name="Price" dataDxfId="17">
       <calculatedColumnFormula>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{32661803-E3A6-42B5-9F3B-102A545567DD}" name="Yen" dataDxfId="0">
+    <tableColumn id="15" xr3:uid="{32661803-E3A6-42B5-9F3B-102A545567DD}" name="Yen" dataDxfId="11">
       <calculatedColumnFormula>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{B604651F-FBED-4C66-90D8-26CA3506AD10}" name="Lead Time" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{71E5A3E7-2DDC-4D5C-9DC1-9D3783AB63E3}" name="Note" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{E824A542-547E-4145-864D-24CA4DB4EBD3}" name="消費税" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{DFAB695D-55D8-4628-9072-10089F337DBD}" name="受注日" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{5EE5CB39-33D3-4188-929E-0C812CC100E2}" name="出荷日" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{B604651F-FBED-4C66-90D8-26CA3506AD10}" name="Lead Time" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{71E5A3E7-2DDC-4D5C-9DC1-9D3783AB63E3}" name="Note" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{E824A542-547E-4145-864D-24CA4DB4EBD3}" name="消費税" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{DFAB695D-55D8-4628-9072-10089F337DBD}" name="受注日" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{5EE5CB39-33D3-4188-929E-0C812CC100E2}" name="出荷日" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A0CBC9AA-8108-43DE-9508-48638514B39D}" name="テーブル6" displayName="テーブル6" ref="A1:L11" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A0CBC9AA-8108-43DE-9508-48638514B39D}" name="テーブル6" displayName="テーブル6" ref="A1:L11" totalsRowShown="0" headerRowDxfId="24">
   <autoFilter ref="A1:L11" xr:uid="{A0CBC9AA-8108-43DE-9508-48638514B39D}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{19CFD427-1401-4365-870F-C15308F7351E}" name="Balloon"/>
@@ -2810,9 +2813,9 @@
     <sortCondition ref="K1:K36"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F16D3331-64F7-4EAC-B32A-50FC4B49BE54}" name="受注日" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{162D6D37-3287-427C-ACB9-1584CB52E535}" name="ミスミ出荷日" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{846787E0-9AEF-4953-B5D9-2C6186063A80}" name="メーカー名" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{F16D3331-64F7-4EAC-B32A-50FC4B49BE54}" name="受注日" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{162D6D37-3287-427C-ACB9-1584CB52E535}" name="ミスミ出荷日" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{846787E0-9AEF-4953-B5D9-2C6186063A80}" name="メーカー名" dataDxfId="19" totalsRowDxfId="18"/>
     <tableColumn id="2" xr3:uid="{6F12422F-1732-4A01-A0B4-10EEAAFE357F}" name="商品型番"/>
     <tableColumn id="8" xr3:uid="{E14E05B1-2076-4CA6-BE48-4C6BB5EB98A9}" name="商品名称"/>
     <tableColumn id="4" xr3:uid="{DC68FDB4-D2ED-47C5-AB1C-914DD1FBC4A5}" name="単価(税別)"/>
@@ -3936,7 +3939,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4014,13 +4017,13 @@
       <c r="F2" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="25">
         <v>25.58</v>
       </c>
       <c r="H2" s="20">
         <v>1</v>
       </c>
-      <c r="I2" s="22">
+      <c r="I2" s="21">
         <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
         <v>25.58</v>
       </c>
@@ -4055,7 +4058,7 @@
       <c r="F3" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="19">
         <v>19.98</v>
       </c>
       <c r="H3" s="9">
@@ -4092,7 +4095,7 @@
       <c r="F4" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="19">
         <v>26.15</v>
       </c>
       <c r="H4" s="9">
@@ -4129,7 +4132,7 @@
       <c r="F5" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="19">
         <v>22.7</v>
       </c>
       <c r="H5" s="9">
@@ -4166,7 +4169,7 @@
       <c r="F6" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="19">
         <v>22.56</v>
       </c>
       <c r="H6" s="9">
@@ -4203,7 +4206,7 @@
       <c r="F7" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="19">
         <v>23.85</v>
       </c>
       <c r="H7" s="9">
@@ -4234,22 +4237,22 @@
       <c r="D8" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="22" t="s">
         <v>21</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="26">
         <v>21</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="22">
         <v>32</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="J8" s="24">
+      <c r="J8" s="23">
         <f>テーブル3[[#This Row],[Unit Price]]*テーブル3[[#This Row],[QTY]]</f>
         <v>672</v>
       </c>
@@ -4276,13 +4279,13 @@
       <c r="F9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="6">
         <v>18</v>
       </c>
       <c r="H9" s="2">
         <v>10</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="24" t="s">
         <v>88</v>
       </c>
       <c r="J9" s="10">

</xml_diff>